<commit_message>
Adding a bunch more games, set stuff up to run batches
</commit_message>
<xml_diff>
--- a/static/data/notes/CountOfGamesPerTeam.xlsx
+++ b/static/data/notes/CountOfGamesPerTeam.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephanos\Documents\Dev\NBAThesis\NBA_Thesis\static\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephanos\Documents\Dev\NBAThesis\NBA_Thesis\static\data\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C05B8DA-3355-49B2-8378-F820178248C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D760692-13E3-47C4-AF02-0257A4CE8204}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-26192" yWindow="-1603" windowWidth="26301" windowHeight="14305" xr2:uid="{632780FF-458B-460E-A361-064A4C562E98}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Spurs</t>
   </si>
@@ -132,12 +132,24 @@
   </si>
   <si>
     <t># of Games</t>
+  </si>
+  <si>
+    <t>Average per Team</t>
+  </si>
+  <si>
+    <t>Max Team</t>
+  </si>
+  <si>
+    <t>Min Team</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -167,8 +179,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,15 +496,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9782A24-87AA-4653-9DB2-385F679BE338}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -516,7 +529,7 @@
         <v>16</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -524,7 +537,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -532,7 +545,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -540,7 +553,7 @@
         <v>13</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -548,7 +561,7 @@
         <v>26</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -564,7 +577,7 @@
         <v>14</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -572,7 +585,7 @@
         <v>17</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -580,7 +593,7 @@
         <v>21</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -588,7 +601,7 @@
         <v>7</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -596,7 +609,7 @@
         <v>1</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -604,7 +617,7 @@
         <v>22</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -628,7 +641,7 @@
         <v>20</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -636,7 +649,7 @@
         <v>12</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -644,7 +657,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -652,7 +665,7 @@
         <v>10</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -660,7 +673,7 @@
         <v>23</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -668,20 +681,23 @@
         <v>18</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>11</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -705,18 +721,24 @@
         <v>9</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>3</v>
       </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>2</v>
       </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -731,7 +753,7 @@
         <v>6</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -740,7 +762,34 @@
       </c>
       <c r="B33">
         <f>SUM(B2:B31)/2</f>
-        <v>29</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1">
+        <f>AVERAGE(B2:B31)</f>
+        <v>3.4666666666666668</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <f>MAX(B2:B31)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <f>MIN(B2:B31)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating, adding annotated col
</commit_message>
<xml_diff>
--- a/static/data/notes/CountOfGamesPerTeam.xlsx
+++ b/static/data/notes/CountOfGamesPerTeam.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephanos\Documents\Dev\NBAThesis\NBA_Thesis\static\data\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D760692-13E3-47C4-AF02-0257A4CE8204}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB75635-C400-4233-98AB-6347D466B7E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26192" yWindow="-1603" windowWidth="26301" windowHeight="14305" xr2:uid="{632780FF-458B-460E-A361-064A4C562E98}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{632780FF-458B-460E-A361-064A4C562E98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Spurs</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>Min Team</t>
+  </si>
+  <si>
+    <t>Annotated</t>
   </si>
 </sst>
 </file>
@@ -148,7 +151,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -181,7 +184,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,51 +499,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9782A24-87AA-4653-9DB2-385F679BE338}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
       <c r="B1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
       <c r="B2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
       <c r="B3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -548,31 +564,37 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
       <c r="B7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
       <c r="B8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -580,15 +602,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="B10">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -596,39 +621,48 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
       <c r="B12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
       <c r="B13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
       <c r="B14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
       <c r="B15">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -636,31 +670,37 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
       <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
       <c r="B18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -668,23 +708,26 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
       <c r="B21">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>18</v>
       </c>
       <c r="B22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -692,103 +735,134 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>11</v>
       </c>
       <c r="B24">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
       <c r="B25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>15</v>
       </c>
       <c r="B26">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>9</v>
       </c>
       <c r="B27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>3</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>2</v>
       </c>
       <c r="B29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
       <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>6</v>
       </c>
       <c r="B31">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
       <c r="B33">
         <f>SUM(B2:B31)/2</f>
-        <v>52</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="C33">
+        <f>SUM(C2:C31)/2</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
       <c r="B34" s="1">
         <f>AVERAGE(B2:B31)</f>
-        <v>3.4666666666666668</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4.1333333333333337</v>
+      </c>
+      <c r="C34" s="1">
+        <f>AVERAGE(C2:C31)</f>
+        <v>1.7647058823529411</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
       <c r="B35">
         <f>MAX(B2:B31)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C35">
+        <f>MAX(C2:C31)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
       <c r="B36">
         <f>MIN(B2:B31)</f>
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <f>MIN(C2:C31)</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>